<commit_message>
updated some aspects of the script and notebooks for testing, ran pipeline and got new data
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D298"/>
+  <dimension ref="A1:D321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6989,6 +6989,512 @@
         </is>
       </c>
     </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Estamos prontos para a Fispal 2025! De 27 a 30 de maio, visite o estande da Copeland e conheça de perto as tecnologias que estão</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Estamos prontos para a Fispal 2025! De 27 a 30 de maio, visite o estande da Copeland e conheça de perto as tecnologias que estão impulsionando a transição energética e acelerando a adoção de...</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333250921482649602</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>In collaboration with North American Sustainable Refrigeration Council (NASRC)’s Natural Refrigerants Webinar Series, Copeland’s</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>In collaboration with North American Sustainable Refrigeration Council (NASRC)’s Natural Refrigerants Webinar Series, Copeland’s Andre Patenaude, CET and Henderson Engineers’ Trevor Jones will...</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333205626983985152</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>CO₂ refrigeration doesn’t have to be intimidating. Whether you’re new to it or building your skillset, Copeland is com</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>CO₂ refrigeration doesn’t have to be intimidating.Whether you’re new to it or building your skillset, Copeland is committed to easing the transition to CO₂ for all skill levels. A recent article by...</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333160353024942080</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Earlier in May, Copeland attended an inspiring #CIBF2025. This year’s event showcased our commitment to reshaping the green</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Earlier in May, Copeland attended an inspiring #CIBF2025. This year’s event showcased our commitment to reshaping the green future of the battery industry. With scalable, forward-thinking solutions,...</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333131185381941249</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Rail heat control in supermarket HVAC-R systems is often overlooked, yet it holds significant potential for energy savings. Join</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Rail heat control in supermarket HVAC-R systems is often overlooked, yet it holds significant potential for energy savings. Join our live event ‘Optimizing Rail Heat Control for Energy Efficient...</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333089370532384771</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>We’re thrilled to share that our #Frascold #compressors were showcased at REFRIGAIR EXPO in Casablanca, thanks to our partn</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>We’re thrilled to share that our #Frascold #compressors were showcased at REFRIGAIR EXPO in Casablanca, thanks to our partnership with #LeFroidPolaire and Tecumseh!An unmissable event for the...</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333057295955689472</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>2025-05-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>DALLMER: Sicherer Umgang mit Wasser – von der Ver- zur Entsorgung</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01.07.2025 um 10:45 - 17:00 Uhr im Dorint Hotel Potsdam Infos zur Live Session Jeder Mensch hat andere Vorstellungen von seinem privaten Traumbad.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.shk-journal.de/news/dallmer-sicherer-umgang-mit-wasser-von-der-ver-zur-entsorgung.html</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>2025-05-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The IPS 8 Air Purger, a highly efficient solution in industrial refrigeration, is now available with propane (R290). Propane is </t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>The IPS 8 Air Purger, a highly efficient solution in industrial refrigeration, is now available with propane (R290). Propane is an environmentally friendly refrigerant with low GWP and high...</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7332675947566907393</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>2025-05-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Copeland partners with Ecozen to aid agriculture sector</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Copeland, a global provider of sustainable heating, cooling, cold chain and industrial solutions, has partnered with Ecozen to develop an innovative solar-powered cold storage system to benefit...</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>http://fnbnews.com/Agriculture/copeland-partners-with-ecozen-to-aidagriculture-sector-82816</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>2025-05-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Copeland Renovates Cudahy Facility for Vilter Industrial Compressors</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> On April 25, Copeland announced the completion of a significant renovation of its Vilter brand’s facility in Cudahy, Wisconsin.</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.ejarn.com/article/detail/88876</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>2025-05-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Designed for liquid, suction, and hot gas lines with ammonia and fluorinated refrigerants, EVRAT 20 valves feature assisted lift</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Designed for liquid, suction, and hot gas lines with ammonia and fluorinated refrigerants, EVRAT 20 valves feature assisted lift and are specially crafted to open and remain open at a pressure drop...</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7331959686415409152</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>2025-05-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Intelligent heating made simple: Danfoss and E.ON One join forces</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Danfoss and E.ON One present an all-in-one solution combining hardware and software that saves up to 30% energy and enables significant CO₂ reductions for both existing and new buildings.</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.danfoss.com/en/about-danfoss/news/cf/intelligent-heating-made-simple-danfoss-and-eon-one-join-forces/</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>2025-05-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">From Pittsburgh (PA) in March, to Irwindale (CA) in April, and most recently St. Paul (MN), our journey with the North American </t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>From Pittsburgh (PA) in March, to Irwindale (CA) in April, and most recently St. Paul (MN), our journey with the North American Sustainable Refrigeration Council (NASRC) in occasion of the Natural...</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7331671573759717377</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>2025-05-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Meet the new Burner Fuel Mobile Pump from Danfoss, engineered for compact mobile heating applications. Whether it’s high-pressur</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Meet the new Burner Fuel Mobile Pump from Danfoss, engineered for compact mobile heating applications. Whether it’s high-pressure cleaners, open-air heaters, or vehicle heating systems, the BFM pump...</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7331634923906269184</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>2025-05-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Intelligent heating made simple: Danfoss and E.ON One join forces</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> May 22, 2025 Danfoss and E.ON One present an all-in-one solution combining hardware and software that saves up to 30% energy and enables significant CO₂ reductions for both existing and new...</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.ejarn.com/article/detail/88836</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Only 5 days left until our RETHINK Live session on retrofitting commercial buildings! Discover how the revised EPBD and Danfoss </t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Only 5 days left until our RETHINK Live session on retrofitting commercial buildings! Discover how the revised EPBD and Danfoss solutions can help you drive energy efficiency and support your...</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7331333039035158528</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Discover a new era of efficiency with Scout, the new AI-powered feature in Copeland Mobile designed to streamline your search fo</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Discover a new era of efficiency with Scout, the new AI-powered feature in Copeland Mobile designed to streamline your search for critical information. Scout delivers HVACR-specific insights sourced...</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7331325526495686656</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Thank you to everyone who joined our recent webinar with ACCA! It was an insightful presentation that covered:</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Thank you to everyone who joined our recent webinar with ACCA! It was an insightful presentation that covered:• Modulation and compressor selection• Why mixing A2L refrigerants and compressors isn’t...</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7331680362739183616</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Hanbell Sales in Q1 2025 have decreased by 19% compared to last year quarter</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Hanbell reports a decline in sales in the first quarter of 2025 (-19% compared to Q1 2024). The sales include both the compressor business, including air and refrigerant compressors, as well as...</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.hanbell.com.cn/financial-reports</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Danfoss and E.ON One are excited to announce a pioneering partnership that offers an all-in-one solution for intelligent heating</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Danfoss and E.ON One are excited to announce a pioneering partnership that offers an all-in-one solution for intelligent heating optimization. By integrating Danfoss’ Leanheat® Building software with...</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7331235301433970692</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Danfoss and E.ON One are excited to announce a pioneering partnership that offers an all-in-one solution for intelligent heating</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Danfoss and E.ON One are excited to announce a pioneering partnership that offers an all-in-one solution for intelligent heating optimization. By integrating Danfoss’s Leanheat® Building software...</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7331235301433970692</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>2025-05-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>The transition to lower-GWP refrigerants can be a source of stress for small grocers who lack the resources and a clear action p</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>The transition to lower-GWP refrigerants can be a source of stress for small grocers who lack the resources and a clear action plan. Unsurprisingly, many are turning to their trusted contractors to...</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7330956149606752256</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>2025-05-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>NeoCharge offers a straightforward solution to enhance the efficiency of both new and existing industrial refrigeration systems.</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>NeoCharge offers a straightforward solution to enhance the efficiency of both new and existing industrial refrigeration systems. By minimizing ammonia charge, it improves system safety and...</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7330917839245082625</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>2025-05-21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated script so that there are seperate methods for article/newsletter content, and made sure that the email recipient list didn't get overwritten during execution
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D321"/>
+  <dimension ref="A1:D336"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7495,6 +7495,336 @@
         </is>
       </c>
     </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>At Copeland, we’re proud to advance sustainable, efficient, and safe production systems for compressors and heat pumps. Our</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>At Copeland, we’re proud to advance sustainable, efficient, and safe production systems for compressors and heat pumps. Our latest interview with Ong-art Veerachartyanukul, General Manager of our...</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7334126665112924160</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SRMTec in 60 seconds: technology, precision, passion. We manufacture screw and piston compressors for refrigeration</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SRMTec in 60 seconds: technology, precision, passion.We manufacture screw and piston compressors for refrigeration, fully designed and made in Italy. Each compressor is tested twice: performance and...</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7334111489491881984</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Our innovative technologies are driving the shift toward sustainable cooling by promoting low-energy consumption and environment</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Our innovative technologies are driving the shift toward sustainable cooling by promoting low-energy consumption and environmentally responsible refrigerants.From cutting-edge compressor designs to...</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7334073630852583424</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>We are excited to announce Andy Baker, MBA as Copeland’s Vice President of Commercial Excellence, a new role within Copeland tha</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>We are excited to announce Andy Baker, MBA as Copeland’s Vice President of Commercial Excellence, a new role within Copeland that will be responsible for leading the global implementation of...</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333915424494952450</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Industrial applications demand reliability, precision and efficiency. Copeland’s innovative Vilter single-screw compression</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Industrial applications demand reliability, precision and efficiency. Copeland’s innovative Vilter single-screw compression technology has proven to be up to the task, delivering superior performance...</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333885283546943490</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>We were thrilled to host the North Florida Refrigerating Engineers &amp; Technicians Association (RETA) - Official Page Chapter meet</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>We were thrilled to host the North Florida Refrigerating Engineers &amp; Technicians Association (RETA) - Official Page Chapter meeting at our #FrascoldUSA office, the first chapter meeting of the...</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333786437319819264</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Mark your calendars for June 12, 2025, at 11 am CET, as we’re hosting an online session – Retrofitting Commercial Buildings</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Mark your calendars for June 12, 2025, at 11 am CET, as we’re hosting an online session – Retrofitting Commercial Buildings with Modulating Room Control. Discover how transitioning from traditional...</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333779205492523008</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Copeland has partnered with Ecozen to deliver solar-powered cold room systems that enable efficient, off-grid refrigeration for </t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Copeland has partnered with Ecozen to deliver solar-powered cold room systems that enable efficient, off-grid refrigeration for the agricultural sector in India. Powered by our variable speed...</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333711238180327426</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Join Our Dynamic Team at Snowman Group!  We are excited to announce the following openings:  Sale</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Join Our Dynamic Team at Snowman Group! We are excited to announce the following openings: Sales Engineer (Food chain industry; Chemical, Oil &amp; Gas industry) After-sales Service EngineerIf you’re...</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333677525769895936</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>2025-05-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Copeland Sensi Equipment Interface Module</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Copeland’s Sensi Equipment Interface Module (Indoor + Outdoor) is a new interface module that eliminates the need for pulling additional HVAC wiring to the thermostat, helping solve installation...</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.phcppros.com/articles/21585-copeland-sensi-equipment-interface-module</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Copeland Thailand Innovation Drives Sustainability, Efficiency, &amp; Safety Wins</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> JARN interviewed Ong-Art Veerachartyanukul, general manager of Copeland’s facility in Rayong, Thailand, who talked about Copeland’s advancing</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.ejarn.com/article/detail/88911</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>Innovations in refrigeration are shaping a more sustainable, efficient future across North America. On June 11 at the ATMOsphere</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Innovations in refrigeration are shaping a more sustainable, efficient future across North America. On June 11 at the ATMOsphere America Summit 2025 in Atlanta, Andre Patenaude, CET, director of...</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333477479543672832</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>NeoCharge is transforming industrial refrigeration by reducing refrigerant charge in both new and existing systems. With easy in</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>NeoCharge is transforming industrial refrigeration by reducing refrigerant charge in both new and existing systems. With easy installation, it offers significant energy savings and increased capacity...</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333454503226077184</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>From Deep-Sea Fishing to End-Point RetailSnowman Refrigeration Technology Locks in Every Bite of Freshness. See you at CHI</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>From Deep-Sea Fishing to End-Point RetailSnowman Refrigeration Technology Locks in Every Bite of Freshness.See you at CHINA (FUZHOU)INTERNATIONAL SEAFOOD &amp; FISHERIES EXPO!  Venue: Fuzhou Strait...</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333431848183730176</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Looking back on an inspiring day: “#Hydrocarbons in the Future of #HVACR” – Padua, May 23. The energ</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Looking back on an inspiring day: “#Hydrocarbons in the Future of #HVACR” – Padua, May 23.The energy, insights and meaningful exchanges of May 23 are still with us.A day that brought together...</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7333415061496958977</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>2025-05-28</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated the api_article call for the newsletter to use the correct topic id for the query params
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D336"/>
+  <dimension ref="A1:D350"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7825,6 +7825,314 @@
         </is>
       </c>
     </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>We are deeply saddened by the passing of Brent Schroeder, a friend, mentor, former colleague and a leader within the air-conditi</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>We are deeply saddened by the passing of Brent Schroeder, a friend, mentor, former colleague and a leader within the air-conditioning and refrigeration industry. Brent spent 35 years at Copeland...</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7335787631324057601</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The next innovation in demanding data center cooling, health care and large chiller applications is here! The Copeland oil-free </t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>The next innovation in demanding data center cooling, health care and large chiller applications is here! The Copeland oil-free centrifugal compressor with frictionless Aero-lift bearing technology...</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7335742157892255744</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Drive performance, efficiency, and innovation with Danfoss at iVT Expo Cologne 2025</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> June 3, 2025 June 2, 2025 — NORDBORG, DENMARK — Danfoss Power Solutions will highlight its latest technologies for off- and on-highway machinery at iVT Expo 2025, June 11-12, in Cologne, Germany.</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.ejarn.com/article/detail/89014</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>DOE Coolerchips’ Peter De Bock joins Eaton as VP of data center energy &amp; cooling</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> As ARPA-E faces dramatic cuts to its budget The head of the Department of Energy’s data center cooling research effort has left for equipment supplier Eaton.</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.datacenterdynamics.com/en/news/doe-coolerchips-peter-de-bock-joins-eaton-as-vp-of-data-center-energy-cooling/</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">TX2-W-G04-Y and TX2-W-G04-Y/H are the Climaveneta branded water source chillers and reversible heat pumps, dedicated to process </t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>TX2-W-G04-Y and TX2-W-G04-Y/H are the Climaveneta branded water source chillers and reversible heat pumps, dedicated to process applications. The range, with capacity from 191 to 2069 kW, has...</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7335636602922110976</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>Romanian hazelnut farm secures €4.6M for expansion</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Dorin Bob, an entrepreneur from Transylvania, Romania, has secured €4.6 million in European funding to expand and modernize a major hazelnut plantation.</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.freshplaza.com/europe/article/9737382/romanian-hazelnut-farm-secures-eur4-6m-for-expansion/</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>On the occasion of China Refrigeration Expo, we interviewed Alvise Dina, Sales Director of #FrascoldChina, right at our booth. I</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>On the occasion of China Refrigeration Expo, we interviewed Alvise Dina, Sales Director of #FrascoldChina, right at our booth.In this short video, Alvise shares insights into #Frascold’s presence in...</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7335597810764894210</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>At Danfoss, we recognize waste heat as a pivotal element in our journey toward decarbonization. Discover how recovering and reus</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>At Danfoss, we recognize waste heat as a pivotal element in our journey toward decarbonization. Discover how recovering and reusing excess heat can significantly enhance energy efficiency and drive...</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7335587321536294913</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>Food retail leaders globally are adopting solutions to meet sustainability and zero-emissions goals, supported by low-GWP refrig</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Food retail leaders globally are adopting solutions to meet sustainability and zero-emissions goals, supported by low-GWP refrigerants that reduce energy waste. Copeland’s CO₂ scroll refrigeration...</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7335545929338392577</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>2025-06-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>Explore Scout, the new AI feature in Copeland Mobile. Scout provides tailored results for Copeland products and continuously imp</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Explore Scout, the new AI feature in Copeland Mobile. Scout provides tailored results for Copeland products and continuously improves through advanced learning. Available 24/7 on mobile and desktop,...</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7335341999199264768</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>2025-06-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>Danfoss Opens Danfoss Nanjing Park</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> On April 23, the opening ceremony for Danfoss Nanjing Park was held in the Nanjing Economic Development Zone.</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.ejarn.com/article/detail/88976</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>2025-06-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>Hanbell Establishes a New Company for Reciprocating Compressors</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Shanghai Hanbell Reciprocating Machinery was officially established with a registered capital of RMB 10 million (about US$ 1.38 million). The business</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.ejarn.com/article/detail/88973</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>2025-06-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Join Jamie Kitchen and guests Jörg Saar and John Broughton in the latest episode of "Taking the Temperature on HVACR." Discover </t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Join Jamie Kitchen and guests Jörg Saar and John Broughton in the latest episode of "Taking the Temperature on HVACR." Discover how temperature and pressure interact within refrigeration systems and...</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/feed/update/urn:li:activity:7334496373041455105</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>Danfoss Delivers AC Drives for Finnish Navy’s Four Corvettes</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Vaasa, Finland-based Danfoss Drives is supplying variable-speed AC drives for the propulsion systems of the Finnish Navy’s four Pohjanmaa-class multi-role corvettes. Part of the Finnish Defense...</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.maritime-executive.com/corporate/danfoss-delivers-ac-drives-for-finnish-navy-s-four-corvettes</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>2025-05-31</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>